<commit_message>
legenda adicionada para as classificações
</commit_message>
<xml_diff>
--- a/Coletor Tweets/ps4.xlsx
+++ b/Coletor Tweets/ps4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbaaa22ba941cb79/Documentos/Segundo_Semestre/CienciaDados/Projetos/Projeto1/Datawitter/CDados_P1/Coletor Tweets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1425" documentId="11_62F829648EEC2C12A7C336D5E9FC1FC65BE8309F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7CF6C48-2DA9-4372-BC4F-5CC282B793BC}"/>
+  <xr:revisionPtr revIDLastSave="1456" documentId="11_62F829648EEC2C12A7C336D5E9FC1FC65BE8309F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69E847C8-B9BF-498E-8796-B69AEE60637E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="1259">
   <si>
     <t>Treinamento</t>
   </si>
@@ -4388,6 +4388,27 @@
   </si>
   <si>
     <t>@fnstatusbr @brasil_fortnite porque não coloca esses camp separado por plataforma ? tem q coloca pc contra ps4 qual é a lógica disso ? 60fps contra 240 140 ??? vocês não pensam não?</t>
+  </si>
+  <si>
+    <t>Relevância</t>
+  </si>
+  <si>
+    <t>Classificação das relevâncias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 -&gt; muito irrelevante                1 -&gt; irrelevante                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 -&gt; muito irrelevante                   1 -&gt; irrelevante                      </t>
+  </si>
+  <si>
+    <t>2 -&gt; neutro                                      3 -&gt; relevante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 -&gt; muito relevante  </t>
+  </si>
+  <si>
+    <t>2 -&gt; neutro                                    3 -&gt; relevante                               4 -&gt; muito relevante</t>
   </si>
 </sst>
 </file>
@@ -4432,7 +4453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4455,6 +4476,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4463,7 +4504,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4475,6 +4516,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -4814,47 +4857,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B752"/>
+  <dimension ref="A1:C752"/>
   <sheetViews>
-    <sheetView topLeftCell="A369" workbookViewId="0">
-      <selection activeCell="B375" sqref="B375"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -4862,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -4870,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4878,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4886,7 +4946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -4894,7 +4954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -4902,7 +4962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -4910,7 +4970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4918,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -4926,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -4934,7 +4994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -4942,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -10841,39 +10901,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B502"/>
+  <dimension ref="A1:C502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G507" sqref="G507"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>752</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>753</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>754</v>
       </c>
@@ -10881,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>755</v>
       </c>
@@ -10889,7 +10963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>756</v>
       </c>
@@ -10897,7 +10971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>757</v>
       </c>
@@ -10905,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>758</v>
       </c>
@@ -10913,7 +10987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>759</v>
       </c>
@@ -10921,7 +10995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>760</v>
       </c>
@@ -10929,7 +11003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>761</v>
       </c>
@@ -10937,7 +11011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>762</v>
       </c>
@@ -10945,7 +11019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>763</v>
       </c>
@@ -10953,7 +11027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>764</v>
       </c>
@@ -10961,7 +11035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>765</v>
       </c>
@@ -10969,7 +11043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>766</v>
       </c>
@@ -14860,5 +14934,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>